<commit_message>
fixed issues and updated gitignore
</commit_message>
<xml_diff>
--- a/data/29/29.xlsx
+++ b/data/29/29.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Sku</t>
   </si>
@@ -33,7 +33,106 @@
     <t>Avg Landed Costs</t>
   </si>
   <si>
+    <t>1B-YHD0-06JY</t>
+  </si>
+  <si>
+    <t>Baby Diaper Caddy Organizer – Nursery Basket with Convenient Leather Handles, Storage Bin – Durable, Portable Changing Table Diaper Storage + Bonus Insulated Wipe Carrier by Cartik™</t>
+  </si>
+  <si>
+    <t>B07C27CG18</t>
+  </si>
+  <si>
+    <t>661708972459</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>EL-NTZN-UZAR</t>
+  </si>
+  <si>
+    <t>Baby Diaper Caddy Organizer – Nursery Basket with Convenient Leather Handles – Durable, Portable Changing Table Diaper Storage (2 Pack)</t>
+  </si>
+  <si>
+    <t>B09PGLKMK9</t>
+  </si>
+  <si>
     <t>child</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>HZ-QVQR-JS29</t>
+  </si>
+  <si>
+    <t>Cartik 2 Pack Backseat Car Organizer for Kids, Babies and Toddlers, with Tablet Holder by iPad Touch Screen, Fit to Baby Stroller, Large Storage, Kick Mat, Back Seat Protector, Organizer eBook</t>
+  </si>
+  <si>
+    <t>B07GNRHN2Q</t>
+  </si>
+  <si>
+    <t>661708972442</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>LD-MT1T-ZNZU</t>
+  </si>
+  <si>
+    <t>Cartik™ Backseat Car Organizer Kids, Babies Toddlers Tablet Holder iPad Touch Screen, Fit to Baby Stroller, Large Storage, Kick Mat, Back Seat Protector, Organizer eBook (one Pack)</t>
+  </si>
+  <si>
+    <t>B076ZJX4SX</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>5L-Y8DM-ULLO</t>
+  </si>
+  <si>
+    <t>Diaper Caddy Organizer (old Diaper Caddy Organizer)</t>
+  </si>
+  <si>
+    <t>B07F1X69HS</t>
+  </si>
+  <si>
+    <t>661708972466</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>JB-GIX4-MKM5</t>
+  </si>
+  <si>
+    <t>O2-WSWS-RNP8</t>
+  </si>
+  <si>
+    <t>Cartik Backseat Car Organizer for Kids, Babies and Toddlers, with Tablet Holder by iPad Touch Screen, Fit to Baby Stroller, Large Storage, Kick Mat, Back Seat Protector, Organizer eBook</t>
+  </si>
+  <si>
+    <t>B07FZQRZZF</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>U1-4AA3-M779</t>
+  </si>
+  <si>
+    <t>Diaper Caddy Organizer</t>
+  </si>
+  <si>
+    <t>B09YFP28G8</t>
   </si>
 </sst>
 </file>
@@ -456,23 +555,83 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -483,7 +642,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -519,13 +678,63 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -572,8 +781,23 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>